<commit_message>
Upload Y4_B2526_General_Surgery_checklist1758178698203_412de898fa38de7e284b58047ef9f3c3397f8d8f5931e4595a3fdbe4844ec332.xlsx via attendance app
</commit_message>
<xml_diff>
--- a/log_history/Y4_B2526_General_Surgery_checklist1758178698203_412de898fa38de7e284b58047ef9f3c3397f8d8f5931e4595a3fdbe4844ec332.xlsx
+++ b/log_history/Y4_B2526_General_Surgery_checklist1758178698203_412de898fa38de7e284b58047ef9f3c3397f8d8f5931e4595a3fdbe4844ec332.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\moham\Desktop\log_history\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\moham\Desktop\log_history\Imported_logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{435DE897-DBA4-4767-BCDF-106006943C02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55D86E25-3ED4-4967-B77B-BF3FFE45B4C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="760" windowWidth="18280" windowHeight="13100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1520" yWindow="1300" windowWidth="18280" windowHeight="13100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Checklist" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="132">
   <si>
     <t>Student ID</t>
   </si>
@@ -410,6 +410,12 @@
   </si>
   <si>
     <t>14/9/2025</t>
+  </si>
+  <si>
+    <t>Edited</t>
+  </si>
+  <si>
+    <t>System</t>
   </si>
 </sst>
 </file>
@@ -794,10 +800,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F121"/>
+  <dimension ref="A1:F122"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D121"/>
+    <sheetView tabSelected="1" topLeftCell="A113" workbookViewId="0">
+      <selection activeCell="E122" sqref="E122:F122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -3226,6 +3232,26 @@
         <v>9</v>
       </c>
     </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A122">
+        <v>200785</v>
+      </c>
+      <c r="B122" t="s">
+        <v>7</v>
+      </c>
+      <c r="C122" t="s">
+        <v>129</v>
+      </c>
+      <c r="D122" s="1">
+        <v>0.460590277777778</v>
+      </c>
+      <c r="E122" t="s">
+        <v>130</v>
+      </c>
+      <c r="F122" t="s">
+        <v>131</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>

</xml_diff>